<commit_message>
Update and fix logic in idle time check
</commit_message>
<xml_diff>
--- a/docs/idle_time_model.xlsx
+++ b/docs/idle_time_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dusti\PycharmProjects\systa\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B008C2C3-3683-466F-8F4D-CB15867D1352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E583152E-952C-4CF7-9940-DBC533238C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4065" yWindow="-16515" windowWidth="28800" windowHeight="15555" xr2:uid="{87030FB5-74AE-40B1-BB74-5DEAAA004307}"/>
+    <workbookView xWindow="0" yWindow="1485" windowWidth="28800" windowHeight="15555" xr2:uid="{87030FB5-74AE-40B1-BB74-5DEAAA004307}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -122,7 +122,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -152,14 +155,16 @@
     <tableColumn id="1" xr3:uid="{B4D02DFD-B003-40C5-92AE-0B7717D505C8}" name="System Time (seconds)"/>
     <tableColumn id="2" xr3:uid="{3C0835A5-655D-4785-89E2-4DA1AE382A6B}" name="User Input At"/>
     <tableColumn id="3" xr3:uid="{D7CB344C-B739-4986-AF45-7D07237ED53A}" name="System Idle Duration"/>
-    <tableColumn id="4" xr3:uid="{7014E490-21F8-4607-9379-4EB7163DF37B}" name="In Idle Period" dataDxfId="2">
+    <tableColumn id="4" xr3:uid="{7014E490-21F8-4607-9379-4EB7163DF37B}" name="In Idle Period" dataDxfId="3">
       <calculatedColumnFormula>Table3[[#This Row],[System Idle Duration]]&gt;user_idle_seconds</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BDEC3584-B6B7-4DBA-A7D7-7A5F310DC6D5}" name="Is Begin Idle Period" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{BDEC3584-B6B7-4DBA-A7D7-7A5F310DC6D5}" name="Is Begin Idle Period" dataDxfId="2">
       <calculatedColumnFormula>AND(Table3[[#This Row],[In Idle Period]], NOT(E3))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{5EEC6D17-545D-400D-B620-FB2B16F851F8}" name="Check Count"/>
-    <tableColumn id="7" xr3:uid="{E8A664ED-F8C4-43F6-BC83-C1DCBC49B618}" name="Return Value" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{5EEC6D17-545D-400D-B620-FB2B16F851F8}" name="Check Count" dataDxfId="0">
+      <calculatedColumnFormula>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F3+1) &lt;= call_count_limit, IF(AND(F3+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F3+1), 0), 0))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{E8A664ED-F8C4-43F6-BC83-C1DCBC49B618}" name="Return Value" dataDxfId="1">
       <calculatedColumnFormula>Table3[[#This Row],[Check Count]]&gt;0</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -467,7 +472,7 @@
   <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,6 +555,7 @@
         <v>0</v>
       </c>
       <c r="F4">
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F3+1) &lt;= call_count_limit, IF(AND(F3+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F3+1), 0), 0))</f>
         <v>0</v>
       </c>
       <c r="G4" t="b">
@@ -580,7 +586,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F4+1) &lt;= call_count_limit, F4+1, 0), 0))</f>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F4+1) &lt;= call_count_limit, IF(AND(F4+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F4+1), 0), 0))</f>
         <v>0</v>
       </c>
       <c r="G5" t="b">
@@ -610,7 +616,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F5+1) &lt;= call_count_limit, F5+1, 0), 0))</f>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F5+1) &lt;= call_count_limit, IF(AND(F5+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F5+1), 0), 0))</f>
         <v>0</v>
       </c>
       <c r="G6" t="b">
@@ -640,7 +646,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F6+1) &lt;= call_count_limit, F6+1, 0), 0))</f>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F6+1) &lt;= call_count_limit, IF(AND(F6+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F6+1), 0), 0))</f>
         <v>0</v>
       </c>
       <c r="G7" t="b">
@@ -670,7 +676,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F7+1) &lt;= call_count_limit, F7+1, 0), 0))</f>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F7+1) &lt;= call_count_limit, IF(AND(F7+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F7+1), 0), 0))</f>
         <v>0</v>
       </c>
       <c r="G8" t="b">
@@ -700,7 +706,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F8+1) &lt;= call_count_limit, F8+1, 0), 0))</f>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F8+1) &lt;= call_count_limit, IF(AND(F8+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F8+1), 0), 0))</f>
         <v>0</v>
       </c>
       <c r="G9" t="b">
@@ -730,7 +736,7 @@
         <v>1</v>
       </c>
       <c r="F10">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F9+1) &lt;= call_count_limit, F9+1, 0), 0))</f>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F9+1) &lt;= call_count_limit, IF(AND(F9+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F9+1), 0), 0))</f>
         <v>1</v>
       </c>
       <c r="G10" t="b">
@@ -760,7 +766,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F10+1) &lt;= call_count_limit, F10+1, 0), 0))</f>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F10+1) &lt;= call_count_limit, IF(AND(F10+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F10+1), 0), 0))</f>
         <v>2</v>
       </c>
       <c r="G11" t="b">
@@ -790,7 +796,7 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F11+1) &lt;= call_count_limit, F11+1, 0), 0))</f>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F11+1) &lt;= call_count_limit, IF(AND(F11+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F11+1), 0), 0))</f>
         <v>0</v>
       </c>
       <c r="G12" t="b">
@@ -820,12 +826,12 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F12+1) &lt;= call_count_limit, F12+1, 0), 0))</f>
-        <v>1</v>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F12+1) &lt;= call_count_limit, IF(AND(F12+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F12+1), 0), 0))</f>
+        <v>0</v>
       </c>
       <c r="G13" t="b">
         <f>Table3[[#This Row],[Check Count]]&gt;0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="4"/>
@@ -850,12 +856,12 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F13+1) &lt;= call_count_limit, F13+1, 0), 0))</f>
-        <v>2</v>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F13+1) &lt;= call_count_limit, IF(AND(F13+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F13+1), 0), 0))</f>
+        <v>0</v>
       </c>
       <c r="G14" t="b">
         <f>Table3[[#This Row],[Check Count]]&gt;0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="4"/>
@@ -880,7 +886,7 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F14+1) &lt;= call_count_limit, F14+1, 0), 0))</f>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F14+1) &lt;= call_count_limit, IF(AND(F14+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F14+1), 0), 0))</f>
         <v>0</v>
       </c>
       <c r="G15" t="b">
@@ -910,7 +916,7 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F15+1) &lt;= call_count_limit, F15+1, 0), 0))</f>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F15+1) &lt;= call_count_limit, IF(AND(F15+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F15+1), 0), 0))</f>
         <v>0</v>
       </c>
       <c r="G16" t="b">
@@ -940,7 +946,7 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F16+1) &lt;= call_count_limit, F16+1, 0), 0))</f>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F16+1) &lt;= call_count_limit, IF(AND(F16+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F16+1), 0), 0))</f>
         <v>0</v>
       </c>
       <c r="G17" t="b">
@@ -970,7 +976,7 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F17+1) &lt;= call_count_limit, F17+1, 0), 0))</f>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F17+1) &lt;= call_count_limit, IF(AND(F17+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F17+1), 0), 0))</f>
         <v>0</v>
       </c>
       <c r="G18" t="b">
@@ -1000,7 +1006,7 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F18+1) &lt;= call_count_limit, F18+1, 0), 0))</f>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F18+1) &lt;= call_count_limit, IF(AND(F18+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F18+1), 0), 0))</f>
         <v>0</v>
       </c>
       <c r="G19" t="b">
@@ -1030,7 +1036,7 @@
         <v>1</v>
       </c>
       <c r="F20">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F19+1) &lt;= call_count_limit, F19+1, 0), 0))</f>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F19+1) &lt;= call_count_limit, IF(AND(F19+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F19+1), 0), 0))</f>
         <v>1</v>
       </c>
       <c r="G20" t="b">
@@ -1060,7 +1066,7 @@
         <v>0</v>
       </c>
       <c r="F21">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F20+1) &lt;= call_count_limit, F20+1, 0), 0))</f>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F20+1) &lt;= call_count_limit, IF(AND(F20+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F20+1), 0), 0))</f>
         <v>2</v>
       </c>
       <c r="G21" t="b">
@@ -1090,7 +1096,7 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F21+1) &lt;= call_count_limit, F21+1, 0), 0))</f>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F21+1) &lt;= call_count_limit, IF(AND(F21+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F21+1), 0), 0))</f>
         <v>0</v>
       </c>
       <c r="G22" t="b">
@@ -1120,12 +1126,12 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F22+1) &lt;= call_count_limit, F22+1, 0), 0))</f>
-        <v>1</v>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F22+1) &lt;= call_count_limit, IF(AND(F22+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F22+1), 0), 0))</f>
+        <v>0</v>
       </c>
       <c r="G23" t="b">
         <f>Table3[[#This Row],[Check Count]]&gt;0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="4"/>
@@ -1150,12 +1156,12 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F23+1) &lt;= call_count_limit, F23+1, 0), 0))</f>
-        <v>2</v>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F23+1) &lt;= call_count_limit, IF(AND(F23+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F23+1), 0), 0))</f>
+        <v>0</v>
       </c>
       <c r="G24" t="b">
         <f>Table3[[#This Row],[Check Count]]&gt;0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="4"/>
@@ -1180,7 +1186,7 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F24+1) &lt;= call_count_limit, F24+1, 0), 0))</f>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F24+1) &lt;= call_count_limit, IF(AND(F24+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F24+1), 0), 0))</f>
         <v>0</v>
       </c>
       <c r="G25" t="b">
@@ -1210,7 +1216,7 @@
         <v>0</v>
       </c>
       <c r="F26">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F25+1) &lt;= call_count_limit, F25+1, 0), 0))</f>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F25+1) &lt;= call_count_limit, IF(AND(F25+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F25+1), 0), 0))</f>
         <v>0</v>
       </c>
       <c r="G26" t="b">
@@ -1240,7 +1246,7 @@
         <v>0</v>
       </c>
       <c r="F27">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F26+1) &lt;= call_count_limit, F26+1, 0), 0))</f>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F26+1) &lt;= call_count_limit, IF(AND(F26+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F26+1), 0), 0))</f>
         <v>0</v>
       </c>
       <c r="G27" t="b">
@@ -1270,7 +1276,7 @@
         <v>0</v>
       </c>
       <c r="F28">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F27+1) &lt;= call_count_limit, F27+1, 0), 0))</f>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F27+1) &lt;= call_count_limit, IF(AND(F27+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F27+1), 0), 0))</f>
         <v>0</v>
       </c>
       <c r="G28" t="b">
@@ -1300,7 +1306,7 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F28+1) &lt;= call_count_limit, F28+1, 0), 0))</f>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F28+1) &lt;= call_count_limit, IF(AND(F28+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F28+1), 0), 0))</f>
         <v>0</v>
       </c>
       <c r="G29" t="b">
@@ -1330,7 +1336,7 @@
         <v>1</v>
       </c>
       <c r="F30">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F29+1) &lt;= call_count_limit, F29+1, 0), 0))</f>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F29+1) &lt;= call_count_limit, IF(AND(F29+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F29+1), 0), 0))</f>
         <v>1</v>
       </c>
       <c r="G30" t="b">
@@ -1360,7 +1366,7 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F30+1) &lt;= call_count_limit, F30+1, 0), 0))</f>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F30+1) &lt;= call_count_limit, IF(AND(F30+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F30+1), 0), 0))</f>
         <v>2</v>
       </c>
       <c r="G31" t="b">
@@ -1390,7 +1396,7 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F31+1) &lt;= call_count_limit, F31+1, 0), 0))</f>
+        <f>IF(AND(Table3[[#This Row],[In Idle Period]],Table3[[#This Row],[Is Begin Idle Period]]), 1, IF(Table3[[#This Row],[In Idle Period]], IF((F31+1) &lt;= call_count_limit, IF(AND(F31+1=1, NOT(Table3[[#This Row],[Is Begin Idle Period]])), 0, F31+1), 0), 0))</f>
         <v>0</v>
       </c>
       <c r="G32" t="b">

</xml_diff>